<commit_message>
Updated unit tests to allow python
</commit_message>
<xml_diff>
--- a/ADP Project Rubrics.xlsx
+++ b/ADP Project Rubrics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\adp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B38DC1-A053-4C02-A351-BD579E262FD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8F9CEE6-ADF1-4A1B-B69F-EE5D43203C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="62">
   <si>
     <t>Acceptatiecriteria</t>
   </si>
@@ -647,8 +647,8 @@
   <dimension ref="A1:Y1077"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E109" sqref="E109"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F156" sqref="F156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4758,7 +4758,9 @@
       <c r="E119" s="4">
         <v>0</v>
       </c>
-      <c r="F119" s="4"/>
+      <c r="F119" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
@@ -4795,7 +4797,9 @@
       <c r="E120" s="15">
         <v>1</v>
       </c>
-      <c r="F120" s="15"/>
+      <c r="F120" s="15">
+        <v>1</v>
+      </c>
       <c r="G120" s="15"/>
       <c r="H120" s="15"/>
       <c r="I120" s="15"/>
@@ -4892,7 +4896,9 @@
       <c r="E123" s="4">
         <v>2</v>
       </c>
-      <c r="F123" s="4"/>
+      <c r="F123" s="4">
+        <v>2</v>
+      </c>
       <c r="G123" s="4"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
@@ -4929,7 +4935,9 @@
       <c r="E124" s="15">
         <v>0</v>
       </c>
-      <c r="F124" s="15"/>
+      <c r="F124" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="G124" s="15"/>
       <c r="H124" s="15"/>
       <c r="I124" s="15"/>
@@ -4966,7 +4974,9 @@
       <c r="E125" s="15">
         <v>1</v>
       </c>
-      <c r="F125" s="15"/>
+      <c r="F125" s="15">
+        <v>1</v>
+      </c>
       <c r="G125" s="15"/>
       <c r="H125" s="15"/>
       <c r="I125" s="15"/>
@@ -5772,7 +5782,9 @@
       <c r="E149" s="4">
         <v>0</v>
       </c>
-      <c r="F149" s="4"/>
+      <c r="F149" s="4" t="s">
+        <v>61</v>
+      </c>
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -5809,7 +5821,9 @@
       <c r="E150" s="15">
         <v>1</v>
       </c>
-      <c r="F150" s="15"/>
+      <c r="F150" s="15">
+        <v>1</v>
+      </c>
       <c r="G150" s="15"/>
       <c r="H150" s="15"/>
       <c r="I150" s="15"/>
@@ -5906,7 +5920,9 @@
       <c r="E153" s="4">
         <v>2</v>
       </c>
-      <c r="F153" s="4"/>
+      <c r="F153" s="4">
+        <v>2</v>
+      </c>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
@@ -5943,7 +5959,9 @@
       <c r="E154" s="15">
         <v>0</v>
       </c>
-      <c r="F154" s="15"/>
+      <c r="F154" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="G154" s="15"/>
       <c r="H154" s="15"/>
       <c r="I154" s="15"/>
@@ -5980,7 +5998,9 @@
       <c r="E155" s="15">
         <v>1</v>
       </c>
-      <c r="F155" s="15"/>
+      <c r="F155" s="15">
+        <v>1</v>
+      </c>
       <c r="G155" s="15"/>
       <c r="H155" s="15"/>
       <c r="I155" s="15"/>

</xml_diff>